<commit_message>
Added some Winbond parts
</commit_message>
<xml_diff>
--- a/Altium/DB.xlsx
+++ b/Altium/DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Repos\LIBS\Altium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1CE056-B605-408F-9225-5BF21D9CF228}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A067DA39-8702-42BD-890A-A1019D6FC1DB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="38625" windowHeight="21225" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6544" uniqueCount="2199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6582" uniqueCount="2211">
   <si>
     <t>Part Number</t>
   </si>
@@ -6630,6 +6630,42 @@
   </si>
   <si>
     <t>TI60F225C4</t>
+  </si>
+  <si>
+    <t>YAG1346CT-ND</t>
+  </si>
+  <si>
+    <t>RT0402BRD0710KL</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 0.1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>256-W958D8NBYA5ITRCT-ND</t>
+  </si>
+  <si>
+    <t>Winbond Electronics</t>
+  </si>
+  <si>
+    <t>W958D8NBYA5I TR</t>
+  </si>
+  <si>
+    <t>256MB HYPERRAM X8, 200MHZ, IND T</t>
+  </si>
+  <si>
+    <t>W958D8NBYAxx</t>
+  </si>
+  <si>
+    <t>256-W25Q64JWSSIQ-ND</t>
+  </si>
+  <si>
+    <t>W25Q64JWSSIQ</t>
+  </si>
+  <si>
+    <t>IC FLASH 64MBIT SPI/QUAD 8SOIC</t>
+  </si>
+  <si>
+    <t>BGA24C100P5X5_600X800X120</t>
   </si>
 </sst>
 </file>
@@ -29494,11 +29530,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N147"/>
+  <dimension ref="A1:N148"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C154" sqref="C154"/>
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E152" sqref="E152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35543,6 +35579,47 @@
       </c>
       <c r="N147" s="2" t="s">
         <v>2175</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>2200</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="E148" s="2" t="s">
+        <v>2201</v>
+      </c>
+      <c r="F148" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="H148" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I148" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="J148" s="4" t="s">
+        <v>1558</v>
+      </c>
+      <c r="K148" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="L148" s="2" t="s">
+        <v>2200</v>
+      </c>
+      <c r="M148" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N148" s="2" t="s">
+        <v>2199</v>
       </c>
     </row>
   </sheetData>
@@ -38834,11 +38911,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N141"/>
+  <dimension ref="A1:N144"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F145" sqref="F145"/>
+      <selection pane="bottomLeft" activeCell="E151" sqref="E151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43817,6 +43894,87 @@
       </c>
       <c r="L141" s="2" t="s">
         <v>2195</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>2204</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>2204</v>
+      </c>
+      <c r="C142" t="s">
+        <v>2206</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>2205</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>2210</v>
+      </c>
+      <c r="H142" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I142" s="2" t="s">
+        <v>2203</v>
+      </c>
+      <c r="J142" s="2" t="s">
+        <v>2204</v>
+      </c>
+      <c r="K142" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L142" s="2" t="s">
+        <v>2202</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>2208</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>2208</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>2208</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>2209</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="H143" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I143" s="2" t="s">
+        <v>2203</v>
+      </c>
+      <c r="J143" s="2" t="s">
+        <v>2208</v>
+      </c>
+      <c r="K143" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L143" s="2" t="s">
+        <v>2207</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D144" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H144" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K144" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RTL8211, bunch of passives
</commit_message>
<xml_diff>
--- a/Altium/DB.xlsx
+++ b/Altium/DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Repos\LIBS\Altium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A067DA39-8702-42BD-890A-A1019D6FC1DB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6873351A-1191-4BB9-9B29-D0798B3E6B3F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="38625" windowHeight="21225" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="38625" windowHeight="21225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6582" uniqueCount="2211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6668" uniqueCount="2244">
   <si>
     <t>Part Number</t>
   </si>
@@ -6666,6 +6666,105 @@
   </si>
   <si>
     <t>BGA24C100P5X5_600X800X120</t>
+  </si>
+  <si>
+    <t>RTL8211F</t>
+  </si>
+  <si>
+    <t>RTL8211F-CG</t>
+  </si>
+  <si>
+    <t>Phy 1-CH 10MBPS/100MBPS/1GBPS 3.3V 40-PIN QFN Ep</t>
+  </si>
+  <si>
+    <t>Realtek</t>
+  </si>
+  <si>
+    <t>QFN40P500X500X90_HS-41N</t>
+  </si>
+  <si>
+    <t>553-1852-ND</t>
+  </si>
+  <si>
+    <t>J0G-0003NL</t>
+  </si>
+  <si>
+    <t>PULSE_J0G-0003NL</t>
+  </si>
+  <si>
+    <t>311-510JRCT-ND</t>
+  </si>
+  <si>
+    <t>510</t>
+  </si>
+  <si>
+    <t>RC0402JR-07510RL</t>
+  </si>
+  <si>
+    <t>RES 510 OHM 5% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>490-5203-1-ND</t>
+  </si>
+  <si>
+    <t>1.3A</t>
+  </si>
+  <si>
+    <t>120 Ohms @ 100 MHz</t>
+  </si>
+  <si>
+    <t>Bead</t>
+  </si>
+  <si>
+    <t>FERRITE BEAD 120 OHM 0402 1LN</t>
+  </si>
+  <si>
+    <t>BLM15PD121SN1D</t>
+  </si>
+  <si>
+    <t>INDC1005X05N</t>
+  </si>
+  <si>
+    <t>490-6700-1-ND</t>
+  </si>
+  <si>
+    <t>1 A</t>
+  </si>
+  <si>
+    <t>LQM2HPN2R2MJ0L</t>
+  </si>
+  <si>
+    <t>150mOhm</t>
+  </si>
+  <si>
+    <t>FIXED IND 2.2UH 1A 150 MOHM SMD</t>
+  </si>
+  <si>
+    <t>INDC2520X12N</t>
+  </si>
+  <si>
+    <t>27pF</t>
+  </si>
+  <si>
+    <t>311-1019-1-ND</t>
+  </si>
+  <si>
+    <t>CC0402JRNPO9BN270</t>
+  </si>
+  <si>
+    <t>CAP CER 27PF 50V C0G/NPO 0402</t>
+  </si>
+  <si>
+    <t>311-1.50KLRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0402FR-071K5L</t>
+  </si>
+  <si>
+    <t>RES 1.5K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>1.5k</t>
   </si>
 </sst>
 </file>
@@ -24915,10 +25014,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P97"/>
+  <dimension ref="A1:P98"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F104" sqref="F104"/>
+    <sheetView topLeftCell="A42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29514,6 +29613,53 @@
         <v>2115</v>
       </c>
     </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="s">
+        <v>2238</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>531</v>
+      </c>
+      <c r="E98" s="6" t="s">
+        <v>2239</v>
+      </c>
+      <c r="F98" s="6" t="s">
+        <v>835</v>
+      </c>
+      <c r="H98" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I98" s="6" t="s">
+        <v>2236</v>
+      </c>
+      <c r="J98" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="K98" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="L98" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="M98" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="N98" s="17" t="s">
+        <v>2238</v>
+      </c>
+      <c r="O98" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P98" s="6" t="s">
+        <v>2237</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:P43">
     <sortCondition ref="F2:F43"/>
@@ -29530,11 +29676,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N148"/>
+  <dimension ref="A1:N150"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E152" sqref="E152"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L153" sqref="L153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35622,6 +35768,88 @@
         <v>2199</v>
       </c>
     </row>
+    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
+        <v>2221</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>2222</v>
+      </c>
+      <c r="F149" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="H149" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I149" s="6" t="s">
+        <v>2220</v>
+      </c>
+      <c r="J149" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K149" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="L149" s="2" t="s">
+        <v>2221</v>
+      </c>
+      <c r="M149" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N149" s="2" t="s">
+        <v>2219</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>2241</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>2242</v>
+      </c>
+      <c r="F150" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="H150" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I150" s="6" t="s">
+        <v>2243</v>
+      </c>
+      <c r="J150" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K150" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="L150" s="2" t="s">
+        <v>2241</v>
+      </c>
+      <c r="M150" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N150" s="2" t="s">
+        <v>2240</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -35635,29 +35863,29 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="1025" width="9" style="23" customWidth="1"/>
     <col min="1026" max="16384" width="8.85546875" style="23"/>
   </cols>
@@ -35805,7 +36033,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>50</v>
+        <v>2226</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>531</v>
@@ -36020,7 +36248,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>50</v>
+        <v>2226</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>531</v>
@@ -36061,7 +36289,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>50</v>
+        <v>2226</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>531</v>
@@ -36190,7 +36418,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>50</v>
+        <v>2226</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>531</v>
@@ -36663,11 +36891,99 @@
         <v>1788</v>
       </c>
     </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>2228</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>2226</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>2227</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>2229</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>2225</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>2224</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>2228</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>2223</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>2232</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>2234</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>2235</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>1287</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>2233</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>2231</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>2232</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>2230</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -38913,9 +39229,9 @@
   </sheetPr>
   <dimension ref="A1:N144"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E151" sqref="E151"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F150" sqref="F150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38923,7 +39239,7 @@
     <col min="1" max="2" width="27.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
@@ -43967,14 +44283,32 @@
       </c>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>2212</v>
+      </c>
+      <c r="B144" t="s">
+        <v>2212</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>2211</v>
+      </c>
       <c r="D144" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="E144" s="2" t="s">
+        <v>2213</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>2215</v>
+      </c>
       <c r="H144" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K144" s="2" t="s">
-        <v>17</v>
+      <c r="I144" s="2" t="s">
+        <v>2214</v>
+      </c>
+      <c r="J144" t="s">
+        <v>2212</v>
       </c>
     </row>
   </sheetData>
@@ -43990,11 +44324,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45324,6 +45658,41 @@
       </c>
       <c r="H40" t="s">
         <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>2217</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>2217</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>2217</v>
+      </c>
+      <c r="D41" t="s">
+        <v>100</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>2218</v>
+      </c>
+      <c r="H41" t="s">
+        <v>99</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>2217</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>2216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update with some bolometers
</commit_message>
<xml_diff>
--- a/Altium/DB.xlsx
+++ b/Altium/DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Repos\LIBS\Altium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C924DA24-152C-4AC0-BFC5-05A91450E7B8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18ECDAD7-1714-49FA-8600-963C56AC4499}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="38625" windowHeight="21225" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6900" uniqueCount="2332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6988" uniqueCount="2369">
   <si>
     <t>Part Number</t>
   </si>
@@ -7029,6 +7029,117 @@
   </si>
   <si>
     <t>CONN FFC/FPC BOTTOM 40P .5MM R/A</t>
+  </si>
+  <si>
+    <t>9774040360</t>
+  </si>
+  <si>
+    <t>Standoff</t>
+  </si>
+  <si>
+    <t>ROUND STANDOFF M3X0.5 STEEL 4MM</t>
+  </si>
+  <si>
+    <t>9774040360R</t>
+  </si>
+  <si>
+    <t>732-5271-1-ND</t>
+  </si>
+  <si>
+    <t>JEDEC_DDR4_SODIMM_SKT_STD_H5.2</t>
+  </si>
+  <si>
+    <t>DDR4 SODIMM 260P 5.2H STD</t>
+  </si>
+  <si>
+    <t>Connector P260 MH</t>
+  </si>
+  <si>
+    <t>2309409-2</t>
+  </si>
+  <si>
+    <t>A141326CT-ND</t>
+  </si>
+  <si>
+    <t>Connector NGFF M.2 Key E</t>
+  </si>
+  <si>
+    <t>Connector NGFF M.2 Key B</t>
+  </si>
+  <si>
+    <t>PCI Express/PCI Connectors M.2 0.5PITCH 4.2H KEY E 10U AU</t>
+  </si>
+  <si>
+    <t>571-1-2199230-1</t>
+  </si>
+  <si>
+    <t>1-2199230-1</t>
+  </si>
+  <si>
+    <t>TE_1-2199230-1</t>
+  </si>
+  <si>
+    <t>TE_1-2199230-0</t>
+  </si>
+  <si>
+    <t>PCI Express/PCI Connectors M.2 0.5PITCH 4.2H KEY B 10U AU</t>
+  </si>
+  <si>
+    <t>1-2199230-0</t>
+  </si>
+  <si>
+    <t>571-1-2199230-0</t>
+  </si>
+  <si>
+    <t>Connector P50</t>
+  </si>
+  <si>
+    <t>26-DF12NB(4.0)-50DP-0.5V(51)CT-ND</t>
+  </si>
+  <si>
+    <t>DF12NB(4.0)-50DP-0.5V(51)</t>
+  </si>
+  <si>
+    <t>HIROSE_DF12NB(4.0)-50DP-0.5V</t>
+  </si>
+  <si>
+    <t>HIROSE_DF12NB-50DS-0.5V</t>
+  </si>
+  <si>
+    <t>DF12NB-50DS-0.5V(51)</t>
+  </si>
+  <si>
+    <t>CONN RCPT 50POS SMD GOLD</t>
+  </si>
+  <si>
+    <t>CONN HDR 50POS SMD GOLD</t>
+  </si>
+  <si>
+    <t>26-DF12NB-50DS-0.5V(51)CT-ND</t>
+  </si>
+  <si>
+    <t>MOLEX_430451027</t>
+  </si>
+  <si>
+    <t>WM7488-ND</t>
+  </si>
+  <si>
+    <t>0430451027</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 10POS 3MM</t>
+  </si>
+  <si>
+    <t>AMPHENOL_94152-088LF</t>
+  </si>
+  <si>
+    <t>94152-088LF</t>
+  </si>
+  <si>
+    <t>CONN MOD JACK 8P8C VERT SHIELDED</t>
+  </si>
+  <si>
+    <t>609-1072-ND</t>
   </si>
 </sst>
 </file>
@@ -45143,28 +45254,27 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E55" sqref="E55"/>
+      <selection pane="bottomLeft" activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="32.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="81.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="79.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="30.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="1025" width="9" style="23" customWidth="1"/>
     <col min="1026" max="16384" width="8.85546875" style="23"/>
   </cols>
@@ -46693,6 +46803,251 @@
       </c>
       <c r="L46" s="2" t="s">
         <v>2326</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>2340</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>2340</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>2339</v>
+      </c>
+      <c r="D47" t="s">
+        <v>100</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>2338</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>2337</v>
+      </c>
+      <c r="H47" t="s">
+        <v>99</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>2340</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>2341</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>2346</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>2342</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>2342</v>
+      </c>
+      <c r="D48" t="s">
+        <v>100</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>2344</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>2347</v>
+      </c>
+      <c r="H48" t="s">
+        <v>99</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>2346</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>2345</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>2350</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>2343</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>2343</v>
+      </c>
+      <c r="D49" t="s">
+        <v>100</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>2349</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>2348</v>
+      </c>
+      <c r="H49" t="s">
+        <v>99</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>2350</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>2351</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>2354</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>2354</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>2352</v>
+      </c>
+      <c r="D50" t="s">
+        <v>100</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>2359</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>2355</v>
+      </c>
+      <c r="H50" t="s">
+        <v>99</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>799</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>2354</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>2353</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>2357</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>2357</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>2352</v>
+      </c>
+      <c r="D51" t="s">
+        <v>100</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>2358</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>2356</v>
+      </c>
+      <c r="H51" t="s">
+        <v>99</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>799</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>2357</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>2360</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>2363</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>2363</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D52" t="s">
+        <v>100</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>2364</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>2361</v>
+      </c>
+      <c r="H52" t="s">
+        <v>99</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>2363</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>2362</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>2366</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>2366</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D53" t="s">
+        <v>100</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>2367</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>2365</v>
+      </c>
+      <c r="H53" t="s">
+        <v>99</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="J53" s="2" t="s">
+        <v>2366</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>2368</v>
       </c>
     </row>
   </sheetData>
@@ -46723,7 +47078,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47221,23 +47576,23 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="8.85546875" style="23"/>
   </cols>
   <sheetData>
@@ -47541,10 +47896,39 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
+      <c r="A11" t="s">
+        <v>2335</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2335</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2333</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>531</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>2334</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>2332</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>2335</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>2336</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12"/>

</xml_diff>

<commit_message>
DDR3 symbol library assignment fix
</commit_message>
<xml_diff>
--- a/Altium/DB.xlsx
+++ b/Altium/DB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Repos\LIBS\Altium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809407DD-B886-4589-B9B7-E61B3B9C7470}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA3181A-07BA-47DE-829A-3398B979DC4F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="495" yWindow="2835" windowWidth="31515" windowHeight="15885" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43439,8 +43439,8 @@
   <dimension ref="A1:N196"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I196" sqref="I196"/>
+      <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D198" sqref="D198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50178,7 +50178,7 @@
         <v>2874</v>
       </c>
       <c r="D196" t="s">
-        <v>19</v>
+        <v>531</v>
       </c>
       <c r="E196" t="s">
         <v>2876</v>

</xml_diff>